<commit_message>
LRs and Semester Project Updates
</commit_message>
<xml_diff>
--- a/ad_viz_plotval_data_1999.xlsx
+++ b/ad_viz_plotval_data_1999.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81956bbec37a5cfd/Documents/ISAT 420/GitHub/ISAT420_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{17D0F278-3E6E-417F-9A47-8937B790515A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:40009_{17D0F278-3E6E-417F-9A47-8937B790515A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C76901F7-D510-44D0-889A-A2B03F5B5CF6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="768" yWindow="552" windowWidth="21372" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ad_viz_plotval_data_60371301" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -115,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -971,17 +987,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="32.33203125" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" customWidth="1"/>
+    <col min="19" max="19" width="12.77734375" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -1048,131 +1080,17 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>36163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>41.8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2">
-        <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>100</v>
-      </c>
-      <c r="K2">
-        <v>88101</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2">
-        <v>31080</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T2">
-        <v>-118.21071000000001</v>
+        <v>36161</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>36166</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>67.7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3">
-        <v>157</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <v>88101</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3">
-        <v>31080</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T3">
-        <v>-118.21071000000001</v>
+        <v>36162</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>36172</v>
+        <v>36163</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1184,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>42</v>
+        <v>41.8</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
@@ -1234,131 +1152,23 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>36178</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>44.1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5">
-        <v>122</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>100</v>
-      </c>
-      <c r="K5">
-        <v>88101</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5">
-        <v>31080</v>
-      </c>
-      <c r="N5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" t="s">
-        <v>29</v>
-      </c>
-      <c r="S5">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T5">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36164</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>36184</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>11.7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6">
-        <v>88101</v>
-      </c>
-      <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6">
-        <v>31080</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S6">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T6">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36165</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>36187</v>
+        <v>36166</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -1370,13 +1180,13 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>16.5</v>
+        <v>67.7</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
@@ -1420,317 +1230,47 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>36193</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8">
-        <v>68</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>100</v>
-      </c>
-      <c r="K8">
-        <v>88101</v>
-      </c>
-      <c r="L8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8">
-        <v>31080</v>
-      </c>
-      <c r="N8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T8">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36167</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>36196</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>20.2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
-      </c>
-      <c r="K9">
-        <v>88101</v>
-      </c>
-      <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9">
-        <v>31080</v>
-      </c>
-      <c r="N9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T9">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36168</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>36199</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>14.4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>100</v>
-      </c>
-      <c r="K10">
-        <v>88101</v>
-      </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10">
-        <v>31080</v>
-      </c>
-      <c r="N10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T10">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36169</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>36202</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>28.7</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11">
-        <v>86</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>100</v>
-      </c>
-      <c r="K11">
-        <v>88101</v>
-      </c>
-      <c r="L11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11">
-        <v>31080</v>
-      </c>
-      <c r="N11" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" t="s">
-        <v>29</v>
-      </c>
-      <c r="S11">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T11">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36170</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>36205</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>25.9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12">
-        <v>80</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>100</v>
-      </c>
-      <c r="K12">
-        <v>88101</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12">
-        <v>31080</v>
-      </c>
-      <c r="N12" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T12">
-        <v>-118.21071000000001</v>
-      </c>
+        <v>36171</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>36208</v>
+        <v>36172</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1742,13 +1282,13 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>35.4</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
@@ -1792,7 +1332,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>36211</v>
+        <v>36178</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1804,13 +1344,13 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>34.799999999999997</v>
+        <v>44.1</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
@@ -1854,7 +1394,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>36214</v>
+        <v>36184</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -1866,13 +1406,13 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>21.6</v>
+        <v>11.7</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
       <c r="G15">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
@@ -1916,7 +1456,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>36217</v>
+        <v>36187</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -1928,13 +1468,13 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>19.8</v>
+        <v>16.5</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
       </c>
       <c r="G16">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
         <v>23</v>
@@ -1978,7 +1518,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>36220</v>
+        <v>36193</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
@@ -1990,13 +1530,13 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>37.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
       </c>
       <c r="G17">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
         <v>23</v>
@@ -2040,7 +1580,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>36226</v>
+        <v>36196</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -2052,13 +1592,13 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>10.5</v>
+        <v>20.2</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
       <c r="G18">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
         <v>23</v>
@@ -2102,7 +1642,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>36229</v>
+        <v>36199</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -2164,7 +1704,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>36232</v>
+        <v>36202</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -2176,13 +1716,13 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>36.299999999999997</v>
+        <v>28.7</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
       </c>
       <c r="G20">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="H20" t="s">
         <v>23</v>
@@ -2226,7 +1766,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>36235</v>
+        <v>36205</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -2238,13 +1778,13 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>20.2</v>
+        <v>25.9</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
       <c r="G21">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H21" t="s">
         <v>23</v>
@@ -2288,7 +1828,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>36238</v>
+        <v>36208</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -2300,13 +1840,13 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>20.5</v>
+        <v>35.4</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="G22">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="H22" t="s">
         <v>23</v>
@@ -2350,7 +1890,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>36247</v>
+        <v>36211</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -2362,13 +1902,13 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>27.7</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="G23">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
         <v>23</v>
@@ -2412,7 +1952,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>36250</v>
+        <v>36214</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
@@ -2424,13 +1964,13 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>12.1</v>
+        <v>21.6</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="G24">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
         <v>23</v>
@@ -2474,7 +2014,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>36253</v>
+        <v>36217</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -2486,13 +2026,13 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>13.6</v>
+        <v>19.8</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
       </c>
       <c r="G25">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="H25" t="s">
         <v>23</v>
@@ -2536,7 +2076,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>36256</v>
+        <v>36220</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
@@ -2548,13 +2088,13 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <v>10.6</v>
+        <v>37.1</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
       </c>
       <c r="G26">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="H26" t="s">
         <v>23</v>
@@ -2598,7 +2138,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>36259</v>
+        <v>36226</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
@@ -2610,13 +2150,13 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="F27" t="s">
         <v>22</v>
       </c>
       <c r="G27">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H27" t="s">
         <v>23</v>
@@ -2660,7 +2200,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>36265</v>
+        <v>36229</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
@@ -2672,13 +2212,13 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>53.2</v>
+        <v>14.4</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
       </c>
       <c r="G28">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="H28" t="s">
         <v>23</v>
@@ -2722,7 +2262,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>36268</v>
+        <v>36232</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
@@ -2734,13 +2274,13 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>32.9</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
       </c>
       <c r="G29">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="H29" t="s">
         <v>23</v>
@@ -2784,7 +2324,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>36271</v>
+        <v>36235</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
@@ -2796,13 +2336,13 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>19</v>
+        <v>20.2</v>
       </c>
       <c r="F30" t="s">
         <v>22</v>
       </c>
       <c r="G30">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H30" t="s">
         <v>23</v>
@@ -2846,7 +2386,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>36274</v>
+        <v>36238</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -2858,13 +2398,13 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <v>17.399999999999999</v>
+        <v>20.5</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
       </c>
       <c r="G31">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H31" t="s">
         <v>23</v>
@@ -2908,7 +2448,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>36277</v>
+        <v>36247</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
@@ -2920,13 +2460,13 @@
         <v>1</v>
       </c>
       <c r="E32">
-        <v>24.2</v>
+        <v>27.7</v>
       </c>
       <c r="F32" t="s">
         <v>22</v>
       </c>
       <c r="G32">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
         <v>23</v>
@@ -2970,7 +2510,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>36280</v>
+        <v>36250</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
@@ -2982,13 +2522,13 @@
         <v>1</v>
       </c>
       <c r="E33">
-        <v>16.100000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
       </c>
       <c r="G33">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H33" t="s">
         <v>23</v>
@@ -3032,7 +2572,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>36283</v>
+        <v>36253</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
@@ -3044,13 +2584,13 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <v>13.2</v>
+        <v>13.6</v>
       </c>
       <c r="F34" t="s">
         <v>22</v>
       </c>
       <c r="G34">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H34" t="s">
         <v>23</v>
@@ -3094,7 +2634,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>36286</v>
+        <v>36256</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
@@ -3106,13 +2646,13 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <v>27.2</v>
+        <v>10.6</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
       </c>
       <c r="G35">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="H35" t="s">
         <v>23</v>
@@ -3156,7 +2696,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>36289</v>
+        <v>36259</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
@@ -3168,13 +2708,13 @@
         <v>1</v>
       </c>
       <c r="E36">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F36" t="s">
         <v>22</v>
       </c>
       <c r="G36">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="H36" t="s">
         <v>23</v>
@@ -3218,7 +2758,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>36292</v>
+        <v>36265</v>
       </c>
       <c r="B37" t="s">
         <v>20</v>
@@ -3230,13 +2770,13 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <v>26.7</v>
+        <v>53.2</v>
       </c>
       <c r="F37" t="s">
         <v>22</v>
       </c>
       <c r="G37">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="H37" t="s">
         <v>23</v>
@@ -3280,7 +2820,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>36295</v>
+        <v>36268</v>
       </c>
       <c r="B38" t="s">
         <v>20</v>
@@ -3292,13 +2832,13 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <v>15.3</v>
+        <v>32.9</v>
       </c>
       <c r="F38" t="s">
         <v>22</v>
       </c>
       <c r="G38">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="H38" t="s">
         <v>23</v>
@@ -3342,7 +2882,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>36298</v>
+        <v>36271</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
@@ -3354,13 +2894,13 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>15.5</v>
+        <v>19</v>
       </c>
       <c r="F39" t="s">
         <v>22</v>
       </c>
       <c r="G39">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="H39" t="s">
         <v>23</v>
@@ -3404,7 +2944,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>36301</v>
+        <v>36274</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
@@ -3416,13 +2956,13 @@
         <v>1</v>
       </c>
       <c r="E40">
-        <v>14</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
       </c>
       <c r="G40">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H40" t="s">
         <v>23</v>
@@ -3466,7 +3006,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>36304</v>
+        <v>36277</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
@@ -3478,13 +3018,13 @@
         <v>1</v>
       </c>
       <c r="E41">
-        <v>18.3</v>
+        <v>24.2</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
       </c>
       <c r="G41">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="H41" t="s">
         <v>23</v>
@@ -3528,7 +3068,7 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>36307</v>
+        <v>36280</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -3540,13 +3080,13 @@
         <v>1</v>
       </c>
       <c r="E42">
-        <v>34.700000000000003</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
       </c>
       <c r="G42">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
         <v>23</v>
@@ -3590,7 +3130,7 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>36310</v>
+        <v>36283</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
@@ -3602,13 +3142,13 @@
         <v>1</v>
       </c>
       <c r="E43">
-        <v>10.8</v>
+        <v>13.2</v>
       </c>
       <c r="F43" t="s">
         <v>22</v>
       </c>
       <c r="G43">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H43" t="s">
         <v>23</v>
@@ -3652,7 +3192,7 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>36313</v>
+        <v>36286</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -3664,13 +3204,13 @@
         <v>1</v>
       </c>
       <c r="E44">
-        <v>8.9</v>
+        <v>27.2</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
       </c>
       <c r="G44">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -3714,7 +3254,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>36316</v>
+        <v>36289</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
@@ -3726,13 +3266,13 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <v>14.3</v>
+        <v>20</v>
       </c>
       <c r="F45" t="s">
         <v>22</v>
       </c>
       <c r="G45">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="H45" t="s">
         <v>23</v>
@@ -3776,7 +3316,7 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>36319</v>
+        <v>36292</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
@@ -3788,13 +3328,13 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>17.2</v>
+        <v>26.7</v>
       </c>
       <c r="F46" t="s">
         <v>22</v>
       </c>
       <c r="G46">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="H46" t="s">
         <v>23</v>
@@ -3838,7 +3378,7 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>36322</v>
+        <v>36295</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
@@ -3850,13 +3390,13 @@
         <v>1</v>
       </c>
       <c r="E47">
-        <v>23.3</v>
+        <v>15.3</v>
       </c>
       <c r="F47" t="s">
         <v>22</v>
       </c>
       <c r="G47">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="H47" t="s">
         <v>23</v>
@@ -3900,7 +3440,7 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>36325</v>
+        <v>36298</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
@@ -3912,13 +3452,13 @@
         <v>1</v>
       </c>
       <c r="E48">
-        <v>24.5</v>
+        <v>15.5</v>
       </c>
       <c r="F48" t="s">
         <v>22</v>
       </c>
       <c r="G48">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="H48" t="s">
         <v>23</v>
@@ -3962,7 +3502,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>36328</v>
+        <v>36301</v>
       </c>
       <c r="B49" t="s">
         <v>20</v>
@@ -3974,13 +3514,13 @@
         <v>1</v>
       </c>
       <c r="E49">
-        <v>36.6</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
         <v>22</v>
       </c>
       <c r="G49">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="H49" t="s">
         <v>23</v>
@@ -4024,7 +3564,7 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>36331</v>
+        <v>36304</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -4036,13 +3576,13 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <v>25.4</v>
+        <v>18.3</v>
       </c>
       <c r="F50" t="s">
         <v>22</v>
       </c>
       <c r="G50">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="H50" t="s">
         <v>23</v>
@@ -4086,7 +3626,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>36334</v>
+        <v>36307</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>
@@ -4098,13 +3638,13 @@
         <v>1</v>
       </c>
       <c r="E51">
-        <v>20.5</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="F51" t="s">
         <v>22</v>
       </c>
       <c r="G51">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="H51" t="s">
         <v>23</v>
@@ -4148,7 +3688,7 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>36337</v>
+        <v>36310</v>
       </c>
       <c r="B52" t="s">
         <v>20</v>
@@ -4160,13 +3700,13 @@
         <v>1</v>
       </c>
       <c r="E52">
-        <v>16.2</v>
+        <v>10.8</v>
       </c>
       <c r="F52" t="s">
         <v>22</v>
       </c>
       <c r="G52">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H52" t="s">
         <v>23</v>
@@ -4210,7 +3750,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>36340</v>
+        <v>36313</v>
       </c>
       <c r="B53" t="s">
         <v>20</v>
@@ -4222,13 +3762,13 @@
         <v>1</v>
       </c>
       <c r="E53">
-        <v>22.7</v>
+        <v>8.9</v>
       </c>
       <c r="F53" t="s">
         <v>22</v>
       </c>
       <c r="G53">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="H53" t="s">
         <v>23</v>
@@ -4272,7 +3812,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>36343</v>
+        <v>36316</v>
       </c>
       <c r="B54" t="s">
         <v>20</v>
@@ -4284,13 +3824,13 @@
         <v>1</v>
       </c>
       <c r="E54">
-        <v>9.5</v>
+        <v>14.3</v>
       </c>
       <c r="F54" t="s">
         <v>22</v>
       </c>
       <c r="G54">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H54" t="s">
         <v>23</v>
@@ -4334,7 +3874,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>36346</v>
+        <v>36319</v>
       </c>
       <c r="B55" t="s">
         <v>20</v>
@@ -4346,13 +3886,13 @@
         <v>1</v>
       </c>
       <c r="E55">
-        <v>35.799999999999997</v>
+        <v>17.2</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
       </c>
       <c r="G55">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="H55" t="s">
         <v>23</v>
@@ -4396,7 +3936,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>36349</v>
+        <v>36322</v>
       </c>
       <c r="B56" t="s">
         <v>20</v>
@@ -4408,13 +3948,13 @@
         <v>1</v>
       </c>
       <c r="E56">
-        <v>21.2</v>
+        <v>23.3</v>
       </c>
       <c r="F56" t="s">
         <v>22</v>
       </c>
       <c r="G56">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H56" t="s">
         <v>23</v>
@@ -4458,7 +3998,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>36352</v>
+        <v>36325</v>
       </c>
       <c r="B57" t="s">
         <v>20</v>
@@ -4470,13 +4010,13 @@
         <v>1</v>
       </c>
       <c r="E57">
-        <v>17.600000000000001</v>
+        <v>24.5</v>
       </c>
       <c r="F57" t="s">
         <v>22</v>
       </c>
       <c r="G57">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="H57" t="s">
         <v>23</v>
@@ -4520,7 +4060,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>36355</v>
+        <v>36328</v>
       </c>
       <c r="B58" t="s">
         <v>20</v>
@@ -4532,13 +4072,13 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>17.7</v>
+        <v>36.6</v>
       </c>
       <c r="F58" t="s">
         <v>22</v>
       </c>
       <c r="G58">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="H58" t="s">
         <v>23</v>
@@ -4582,7 +4122,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>36358</v>
+        <v>36331</v>
       </c>
       <c r="B59" t="s">
         <v>20</v>
@@ -4594,13 +4134,13 @@
         <v>1</v>
       </c>
       <c r="E59">
-        <v>15.5</v>
+        <v>25.4</v>
       </c>
       <c r="F59" t="s">
         <v>22</v>
       </c>
       <c r="G59">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="H59" t="s">
         <v>23</v>
@@ -4644,7 +4184,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>36361</v>
+        <v>36334</v>
       </c>
       <c r="B60" t="s">
         <v>20</v>
@@ -4656,13 +4196,13 @@
         <v>1</v>
       </c>
       <c r="E60">
-        <v>11.7</v>
+        <v>20.5</v>
       </c>
       <c r="F60" t="s">
         <v>22</v>
       </c>
       <c r="G60">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="H60" t="s">
         <v>23</v>
@@ -4706,7 +4246,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>36364</v>
+        <v>36337</v>
       </c>
       <c r="B61" t="s">
         <v>20</v>
@@ -4718,13 +4258,13 @@
         <v>1</v>
       </c>
       <c r="E61">
-        <v>13.8</v>
+        <v>16.2</v>
       </c>
       <c r="F61" t="s">
         <v>22</v>
       </c>
       <c r="G61">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H61" t="s">
         <v>23</v>
@@ -4768,7 +4308,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>36367</v>
+        <v>36340</v>
       </c>
       <c r="B62" t="s">
         <v>20</v>
@@ -4780,13 +4320,13 @@
         <v>1</v>
       </c>
       <c r="E62">
-        <v>21.2</v>
+        <v>22.7</v>
       </c>
       <c r="F62" t="s">
         <v>22</v>
       </c>
       <c r="G62">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H62" t="s">
         <v>23</v>
@@ -4830,7 +4370,7 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>36370</v>
+        <v>36343</v>
       </c>
       <c r="B63" t="s">
         <v>20</v>
@@ -4842,13 +4382,13 @@
         <v>1</v>
       </c>
       <c r="E63">
-        <v>14.2</v>
+        <v>9.5</v>
       </c>
       <c r="F63" t="s">
         <v>22</v>
       </c>
       <c r="G63">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="H63" t="s">
         <v>23</v>
@@ -4892,7 +4432,7 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>36373</v>
+        <v>36346</v>
       </c>
       <c r="B64" t="s">
         <v>20</v>
@@ -4904,13 +4444,13 @@
         <v>1</v>
       </c>
       <c r="E64">
-        <v>14.6</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="F64" t="s">
         <v>22</v>
       </c>
       <c r="G64">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H64" t="s">
         <v>23</v>
@@ -4954,7 +4494,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>36376</v>
+        <v>36349</v>
       </c>
       <c r="B65" t="s">
         <v>20</v>
@@ -4966,13 +4506,13 @@
         <v>1</v>
       </c>
       <c r="E65">
-        <v>19.2</v>
+        <v>21.2</v>
       </c>
       <c r="F65" t="s">
         <v>22</v>
       </c>
       <c r="G65">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H65" t="s">
         <v>23</v>
@@ -5016,7 +4556,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>36379</v>
+        <v>36352</v>
       </c>
       <c r="B66" t="s">
         <v>20</v>
@@ -5028,13 +4568,13 @@
         <v>1</v>
       </c>
       <c r="E66">
-        <v>9</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F66" t="s">
         <v>22</v>
       </c>
       <c r="G66">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
@@ -5078,7 +4618,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>36382</v>
+        <v>36355</v>
       </c>
       <c r="B67" t="s">
         <v>20</v>
@@ -5090,13 +4630,13 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>9.8000000000000007</v>
+        <v>17.7</v>
       </c>
       <c r="F67" t="s">
         <v>22</v>
       </c>
       <c r="G67">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="H67" t="s">
         <v>23</v>
@@ -5140,7 +4680,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>36385</v>
+        <v>36358</v>
       </c>
       <c r="B68" t="s">
         <v>20</v>
@@ -5152,13 +4692,13 @@
         <v>1</v>
       </c>
       <c r="E68">
-        <v>17.7</v>
+        <v>15.5</v>
       </c>
       <c r="F68" t="s">
         <v>22</v>
       </c>
       <c r="G68">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H68" t="s">
         <v>23</v>
@@ -5202,7 +4742,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>36388</v>
+        <v>36361</v>
       </c>
       <c r="B69" t="s">
         <v>20</v>
@@ -5214,13 +4754,13 @@
         <v>1</v>
       </c>
       <c r="E69">
-        <v>15</v>
+        <v>11.7</v>
       </c>
       <c r="F69" t="s">
         <v>22</v>
       </c>
       <c r="G69">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H69" t="s">
         <v>23</v>
@@ -5264,7 +4804,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>36391</v>
+        <v>36364</v>
       </c>
       <c r="B70" t="s">
         <v>20</v>
@@ -5276,13 +4816,13 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <v>17.8</v>
+        <v>13.8</v>
       </c>
       <c r="F70" t="s">
         <v>22</v>
       </c>
       <c r="G70">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H70" t="s">
         <v>23</v>
@@ -5326,7 +4866,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>36394</v>
+        <v>36367</v>
       </c>
       <c r="B71" t="s">
         <v>20</v>
@@ -5338,7 +4878,7 @@
         <v>1</v>
       </c>
       <c r="E71">
-        <v>21.1</v>
+        <v>21.2</v>
       </c>
       <c r="F71" t="s">
         <v>22</v>
@@ -5388,7 +4928,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>36397</v>
+        <v>36370</v>
       </c>
       <c r="B72" t="s">
         <v>20</v>
@@ -5400,13 +4940,13 @@
         <v>1</v>
       </c>
       <c r="E72">
-        <v>18.8</v>
+        <v>14.2</v>
       </c>
       <c r="F72" t="s">
         <v>22</v>
       </c>
       <c r="G72">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="H72" t="s">
         <v>23</v>
@@ -5450,7 +4990,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>36400</v>
+        <v>36373</v>
       </c>
       <c r="B73" t="s">
         <v>20</v>
@@ -5462,13 +5002,13 @@
         <v>1</v>
       </c>
       <c r="E73">
-        <v>18.600000000000001</v>
+        <v>14.6</v>
       </c>
       <c r="F73" t="s">
         <v>22</v>
       </c>
       <c r="G73">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H73" t="s">
         <v>23</v>
@@ -5512,7 +5052,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>36403</v>
+        <v>36376</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
@@ -5524,13 +5064,13 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <v>22.2</v>
+        <v>19.2</v>
       </c>
       <c r="F74" t="s">
         <v>22</v>
       </c>
       <c r="G74">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H74" t="s">
         <v>23</v>
@@ -5574,7 +5114,7 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>36406</v>
+        <v>36379</v>
       </c>
       <c r="B75" t="s">
         <v>20</v>
@@ -5586,13 +5126,13 @@
         <v>1</v>
       </c>
       <c r="E75">
-        <v>13.2</v>
+        <v>9</v>
       </c>
       <c r="F75" t="s">
         <v>22</v>
       </c>
       <c r="G75">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H75" t="s">
         <v>23</v>
@@ -5636,7 +5176,7 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>36409</v>
+        <v>36382</v>
       </c>
       <c r="B76" t="s">
         <v>20</v>
@@ -5648,13 +5188,13 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <v>30.2</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
       </c>
       <c r="G76">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="H76" t="s">
         <v>23</v>
@@ -5698,7 +5238,7 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>36412</v>
+        <v>36385</v>
       </c>
       <c r="B77" t="s">
         <v>20</v>
@@ -5710,13 +5250,13 @@
         <v>1</v>
       </c>
       <c r="E77">
-        <v>15.4</v>
+        <v>17.7</v>
       </c>
       <c r="F77" t="s">
         <v>22</v>
       </c>
       <c r="G77">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H77" t="s">
         <v>23</v>
@@ -5760,7 +5300,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>36415</v>
+        <v>36388</v>
       </c>
       <c r="B78" t="s">
         <v>20</v>
@@ -5772,13 +5312,13 @@
         <v>1</v>
       </c>
       <c r="E78">
-        <v>16.100000000000001</v>
+        <v>15</v>
       </c>
       <c r="F78" t="s">
         <v>22</v>
       </c>
       <c r="G78">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H78" t="s">
         <v>23</v>
@@ -5822,7 +5362,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>36418</v>
+        <v>36391</v>
       </c>
       <c r="B79" t="s">
         <v>20</v>
@@ -5834,13 +5374,13 @@
         <v>1</v>
       </c>
       <c r="E79">
-        <v>29.3</v>
+        <v>17.8</v>
       </c>
       <c r="F79" t="s">
         <v>22</v>
       </c>
       <c r="G79">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="H79" t="s">
         <v>23</v>
@@ -5884,7 +5424,7 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>36427</v>
+        <v>36394</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
@@ -5896,13 +5436,13 @@
         <v>1</v>
       </c>
       <c r="E80">
-        <v>35.5</v>
+        <v>21.1</v>
       </c>
       <c r="F80" t="s">
         <v>22</v>
       </c>
       <c r="G80">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="H80" t="s">
         <v>23</v>
@@ -5946,7 +5486,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>36430</v>
+        <v>36397</v>
       </c>
       <c r="B81" t="s">
         <v>20</v>
@@ -5958,13 +5498,13 @@
         <v>1</v>
       </c>
       <c r="E81">
-        <v>20.7</v>
+        <v>18.8</v>
       </c>
       <c r="F81" t="s">
         <v>22</v>
       </c>
       <c r="G81">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H81" t="s">
         <v>23</v>
@@ -6008,7 +5548,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>36433</v>
+        <v>36400</v>
       </c>
       <c r="B82" t="s">
         <v>20</v>
@@ -6020,13 +5560,13 @@
         <v>1</v>
       </c>
       <c r="E82">
-        <v>22.5</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="F82" t="s">
         <v>22</v>
       </c>
       <c r="G82">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H82" t="s">
         <v>23</v>
@@ -6070,7 +5610,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>36436</v>
+        <v>36403</v>
       </c>
       <c r="B83" t="s">
         <v>20</v>
@@ -6082,13 +5622,13 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <v>38.799999999999997</v>
+        <v>22.2</v>
       </c>
       <c r="F83" t="s">
         <v>22</v>
       </c>
       <c r="G83">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="H83" t="s">
         <v>23</v>
@@ -6132,7 +5672,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>36439</v>
+        <v>36406</v>
       </c>
       <c r="B84" t="s">
         <v>20</v>
@@ -6144,13 +5684,13 @@
         <v>1</v>
       </c>
       <c r="E84">
-        <v>11</v>
+        <v>13.2</v>
       </c>
       <c r="F84" t="s">
         <v>22</v>
       </c>
       <c r="G84">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H84" t="s">
         <v>23</v>
@@ -6194,7 +5734,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>36442</v>
+        <v>36409</v>
       </c>
       <c r="B85" t="s">
         <v>20</v>
@@ -6206,13 +5746,13 @@
         <v>1</v>
       </c>
       <c r="E85">
-        <v>24</v>
+        <v>30.2</v>
       </c>
       <c r="F85" t="s">
         <v>22</v>
       </c>
       <c r="G85">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="H85" t="s">
         <v>23</v>
@@ -6256,7 +5796,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>36445</v>
+        <v>36412</v>
       </c>
       <c r="B86" t="s">
         <v>20</v>
@@ -6268,13 +5808,13 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <v>21.5</v>
+        <v>15.4</v>
       </c>
       <c r="F86" t="s">
         <v>22</v>
       </c>
       <c r="G86">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H86" t="s">
         <v>23</v>
@@ -6318,7 +5858,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>36448</v>
+        <v>36415</v>
       </c>
       <c r="B87" t="s">
         <v>20</v>
@@ -6330,13 +5870,13 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>16.3</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="F87" t="s">
         <v>22</v>
       </c>
       <c r="G87">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H87" t="s">
         <v>23</v>
@@ -6380,7 +5920,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>36451</v>
+        <v>36418</v>
       </c>
       <c r="B88" t="s">
         <v>20</v>
@@ -6392,13 +5932,13 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>19.600000000000001</v>
+        <v>29.3</v>
       </c>
       <c r="F88" t="s">
         <v>22</v>
       </c>
       <c r="G88">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="H88" t="s">
         <v>23</v>
@@ -6442,7 +5982,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>36454</v>
+        <v>36427</v>
       </c>
       <c r="B89" t="s">
         <v>20</v>
@@ -6454,13 +5994,13 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>24.4</v>
+        <v>35.5</v>
       </c>
       <c r="F89" t="s">
         <v>22</v>
       </c>
       <c r="G89">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="H89" t="s">
         <v>23</v>
@@ -6504,7 +6044,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>36457</v>
+        <v>36430</v>
       </c>
       <c r="B90" t="s">
         <v>20</v>
@@ -6516,13 +6056,13 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>38.299999999999997</v>
+        <v>20.7</v>
       </c>
       <c r="F90" t="s">
         <v>22</v>
       </c>
       <c r="G90">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="H90" t="s">
         <v>23</v>
@@ -6566,7 +6106,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>36460</v>
+        <v>36433</v>
       </c>
       <c r="B91" t="s">
         <v>20</v>
@@ -6578,13 +6118,13 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>44.4</v>
+        <v>22.5</v>
       </c>
       <c r="F91" t="s">
         <v>22</v>
       </c>
       <c r="G91">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="H91" t="s">
         <v>23</v>
@@ -6628,7 +6168,7 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>36463</v>
+        <v>36436</v>
       </c>
       <c r="B92" t="s">
         <v>20</v>
@@ -6640,13 +6180,13 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <v>20.3</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="F92" t="s">
         <v>22</v>
       </c>
       <c r="G92">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="H92" t="s">
         <v>23</v>
@@ -6690,7 +6230,7 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>36466</v>
+        <v>36439</v>
       </c>
       <c r="B93" t="s">
         <v>20</v>
@@ -6702,13 +6242,13 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <v>49.4</v>
+        <v>11</v>
       </c>
       <c r="F93" t="s">
         <v>22</v>
       </c>
       <c r="G93">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="H93" t="s">
         <v>23</v>
@@ -6752,7 +6292,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>36469</v>
+        <v>36442</v>
       </c>
       <c r="B94" t="s">
         <v>20</v>
@@ -6764,13 +6304,13 @@
         <v>1</v>
       </c>
       <c r="E94">
-        <v>53.7</v>
+        <v>24</v>
       </c>
       <c r="F94" t="s">
         <v>22</v>
       </c>
       <c r="G94">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="H94" t="s">
         <v>23</v>
@@ -6814,7 +6354,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>36472</v>
+        <v>36445</v>
       </c>
       <c r="B95" t="s">
         <v>20</v>
@@ -6826,13 +6366,13 @@
         <v>1</v>
       </c>
       <c r="E95">
-        <v>14.1</v>
+        <v>21.5</v>
       </c>
       <c r="F95" t="s">
         <v>22</v>
       </c>
       <c r="G95">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="H95" t="s">
         <v>23</v>
@@ -6876,7 +6416,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>36475</v>
+        <v>36448</v>
       </c>
       <c r="B96" t="s">
         <v>20</v>
@@ -6888,13 +6428,13 @@
         <v>1</v>
       </c>
       <c r="E96">
-        <v>45</v>
+        <v>16.3</v>
       </c>
       <c r="F96" t="s">
         <v>22</v>
       </c>
       <c r="G96">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="H96" t="s">
         <v>23</v>
@@ -6938,7 +6478,7 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>36478</v>
+        <v>36451</v>
       </c>
       <c r="B97" t="s">
         <v>20</v>
@@ -6950,13 +6490,13 @@
         <v>1</v>
       </c>
       <c r="E97">
-        <v>32.799999999999997</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F97" t="s">
         <v>22</v>
       </c>
       <c r="G97">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="H97" t="s">
         <v>23</v>
@@ -7000,7 +6540,7 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>36481</v>
+        <v>36454</v>
       </c>
       <c r="B98" t="s">
         <v>20</v>
@@ -7012,13 +6552,13 @@
         <v>1</v>
       </c>
       <c r="E98">
-        <v>9.1999999999999993</v>
+        <v>24.4</v>
       </c>
       <c r="F98" t="s">
         <v>22</v>
       </c>
       <c r="G98">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="H98" t="s">
         <v>23</v>
@@ -7062,7 +6602,7 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>36484</v>
+        <v>36457</v>
       </c>
       <c r="B99" t="s">
         <v>20</v>
@@ -7074,13 +6614,13 @@
         <v>1</v>
       </c>
       <c r="E99">
-        <v>28.5</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="F99" t="s">
         <v>22</v>
       </c>
       <c r="G99">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="H99" t="s">
         <v>23</v>
@@ -7124,7 +6664,7 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>36487</v>
+        <v>36460</v>
       </c>
       <c r="B100" t="s">
         <v>20</v>
@@ -7136,13 +6676,13 @@
         <v>1</v>
       </c>
       <c r="E100">
-        <v>21.5</v>
+        <v>44.4</v>
       </c>
       <c r="F100" t="s">
         <v>22</v>
       </c>
       <c r="G100">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="H100" t="s">
         <v>23</v>
@@ -7186,7 +6726,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
-        <v>36490</v>
+        <v>36463</v>
       </c>
       <c r="B101" t="s">
         <v>20</v>
@@ -7198,13 +6738,13 @@
         <v>1</v>
       </c>
       <c r="E101">
-        <v>34.9</v>
+        <v>20.3</v>
       </c>
       <c r="F101" t="s">
         <v>22</v>
       </c>
       <c r="G101">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="H101" t="s">
         <v>23</v>
@@ -7248,7 +6788,7 @@
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>36493</v>
+        <v>36466</v>
       </c>
       <c r="B102" t="s">
         <v>20</v>
@@ -7260,13 +6800,13 @@
         <v>1</v>
       </c>
       <c r="E102">
-        <v>36.299999999999997</v>
+        <v>49.4</v>
       </c>
       <c r="F102" t="s">
         <v>22</v>
       </c>
       <c r="G102">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="H102" t="s">
         <v>23</v>
@@ -7310,7 +6850,7 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>36496</v>
+        <v>36469</v>
       </c>
       <c r="B103" t="s">
         <v>20</v>
@@ -7322,13 +6862,13 @@
         <v>1</v>
       </c>
       <c r="E103">
-        <v>30.5</v>
+        <v>53.7</v>
       </c>
       <c r="F103" t="s">
         <v>22</v>
       </c>
       <c r="G103">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="H103" t="s">
         <v>23</v>
@@ -7372,7 +6912,7 @@
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
-        <v>36499</v>
+        <v>36472</v>
       </c>
       <c r="B104" t="s">
         <v>20</v>
@@ -7384,13 +6924,13 @@
         <v>1</v>
       </c>
       <c r="E104">
-        <v>20</v>
+        <v>14.1</v>
       </c>
       <c r="F104" t="s">
         <v>22</v>
       </c>
       <c r="G104">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="H104" t="s">
         <v>23</v>
@@ -7434,7 +6974,7 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
-        <v>36502</v>
+        <v>36475</v>
       </c>
       <c r="B105" t="s">
         <v>20</v>
@@ -7446,13 +6986,13 @@
         <v>1</v>
       </c>
       <c r="E105">
-        <v>26.9</v>
+        <v>45</v>
       </c>
       <c r="F105" t="s">
         <v>22</v>
       </c>
       <c r="G105">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="H105" t="s">
         <v>23</v>
@@ -7496,7 +7036,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
-        <v>36505</v>
+        <v>36478</v>
       </c>
       <c r="B106" t="s">
         <v>20</v>
@@ -7508,13 +7048,13 @@
         <v>1</v>
       </c>
       <c r="E106">
-        <v>26.1</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F106" t="s">
         <v>22</v>
       </c>
       <c r="G106">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H106" t="s">
         <v>23</v>
@@ -7558,7 +7098,7 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
-        <v>36508</v>
+        <v>36481</v>
       </c>
       <c r="B107" t="s">
         <v>20</v>
@@ -7570,13 +7110,13 @@
         <v>1</v>
       </c>
       <c r="E107">
-        <v>38.700000000000003</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F107" t="s">
         <v>22</v>
       </c>
       <c r="G107">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="H107" t="s">
         <v>23</v>
@@ -7620,7 +7160,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
-        <v>36511</v>
+        <v>36484</v>
       </c>
       <c r="B108" t="s">
         <v>20</v>
@@ -7632,13 +7172,13 @@
         <v>1</v>
       </c>
       <c r="E108">
-        <v>35.200000000000003</v>
+        <v>28.5</v>
       </c>
       <c r="F108" t="s">
         <v>22</v>
       </c>
       <c r="G108">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="H108" t="s">
         <v>23</v>
@@ -7682,7 +7222,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
-        <v>36514</v>
+        <v>36487</v>
       </c>
       <c r="B109" t="s">
         <v>20</v>
@@ -7694,13 +7234,13 @@
         <v>1</v>
       </c>
       <c r="E109">
-        <v>44.2</v>
+        <v>21.5</v>
       </c>
       <c r="F109" t="s">
         <v>22</v>
       </c>
       <c r="G109">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="H109" t="s">
         <v>23</v>
@@ -7744,7 +7284,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
-        <v>36517</v>
+        <v>36490</v>
       </c>
       <c r="B110" t="s">
         <v>20</v>
@@ -7756,13 +7296,13 @@
         <v>1</v>
       </c>
       <c r="E110">
-        <v>31.2</v>
+        <v>34.9</v>
       </c>
       <c r="F110" t="s">
         <v>22</v>
       </c>
       <c r="G110">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H110" t="s">
         <v>23</v>
@@ -7806,63 +7346,621 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
+        <v>36493</v>
+      </c>
+      <c r="B111" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F111" t="s">
+        <v>22</v>
+      </c>
+      <c r="G111">
+        <v>103</v>
+      </c>
+      <c r="H111" t="s">
+        <v>23</v>
+      </c>
+      <c r="I111">
+        <v>1</v>
+      </c>
+      <c r="J111">
+        <v>100</v>
+      </c>
+      <c r="K111">
+        <v>88101</v>
+      </c>
+      <c r="L111" t="s">
+        <v>24</v>
+      </c>
+      <c r="M111">
+        <v>31080</v>
+      </c>
+      <c r="N111" t="s">
+        <v>25</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P111" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q111" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R111" t="s">
+        <v>29</v>
+      </c>
+      <c r="S111">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T111">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>36496</v>
+      </c>
+      <c r="B112" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>30.5</v>
+      </c>
+      <c r="F112" t="s">
+        <v>22</v>
+      </c>
+      <c r="G112">
+        <v>90</v>
+      </c>
+      <c r="H112" t="s">
+        <v>23</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>100</v>
+      </c>
+      <c r="K112">
+        <v>88101</v>
+      </c>
+      <c r="L112" t="s">
+        <v>24</v>
+      </c>
+      <c r="M112">
+        <v>31080</v>
+      </c>
+      <c r="N112" t="s">
+        <v>25</v>
+      </c>
+      <c r="O112" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P112" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q112" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R112" t="s">
+        <v>29</v>
+      </c>
+      <c r="S112">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T112">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>36499</v>
+      </c>
+      <c r="B113" t="s">
+        <v>20</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>20</v>
+      </c>
+      <c r="F113" t="s">
+        <v>22</v>
+      </c>
+      <c r="G113">
+        <v>68</v>
+      </c>
+      <c r="H113" t="s">
+        <v>23</v>
+      </c>
+      <c r="I113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>100</v>
+      </c>
+      <c r="K113">
+        <v>88101</v>
+      </c>
+      <c r="L113" t="s">
+        <v>24</v>
+      </c>
+      <c r="M113">
+        <v>31080</v>
+      </c>
+      <c r="N113" t="s">
+        <v>25</v>
+      </c>
+      <c r="O113" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P113" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R113" t="s">
+        <v>29</v>
+      </c>
+      <c r="S113">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T113">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>36502</v>
+      </c>
+      <c r="B114" t="s">
+        <v>20</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>26.9</v>
+      </c>
+      <c r="F114" t="s">
+        <v>22</v>
+      </c>
+      <c r="G114">
+        <v>82</v>
+      </c>
+      <c r="H114" t="s">
+        <v>23</v>
+      </c>
+      <c r="I114">
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <v>100</v>
+      </c>
+      <c r="K114">
+        <v>88101</v>
+      </c>
+      <c r="L114" t="s">
+        <v>24</v>
+      </c>
+      <c r="M114">
+        <v>31080</v>
+      </c>
+      <c r="N114" t="s">
+        <v>25</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P114" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R114" t="s">
+        <v>29</v>
+      </c>
+      <c r="S114">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T114">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>36505</v>
+      </c>
+      <c r="B115" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>26.1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>22</v>
+      </c>
+      <c r="G115">
+        <v>80</v>
+      </c>
+      <c r="H115" t="s">
+        <v>23</v>
+      </c>
+      <c r="I115">
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>100</v>
+      </c>
+      <c r="K115">
+        <v>88101</v>
+      </c>
+      <c r="L115" t="s">
+        <v>24</v>
+      </c>
+      <c r="M115">
+        <v>31080</v>
+      </c>
+      <c r="N115" t="s">
+        <v>25</v>
+      </c>
+      <c r="O115" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P115" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q115" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R115" t="s">
+        <v>29</v>
+      </c>
+      <c r="S115">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T115">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>36508</v>
+      </c>
+      <c r="B116" t="s">
+        <v>20</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="F116" t="s">
+        <v>22</v>
+      </c>
+      <c r="G116">
+        <v>109</v>
+      </c>
+      <c r="H116" t="s">
+        <v>23</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>100</v>
+      </c>
+      <c r="K116">
+        <v>88101</v>
+      </c>
+      <c r="L116" t="s">
+        <v>24</v>
+      </c>
+      <c r="M116">
+        <v>31080</v>
+      </c>
+      <c r="N116" t="s">
+        <v>25</v>
+      </c>
+      <c r="O116" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P116" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q116" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R116" t="s">
+        <v>29</v>
+      </c>
+      <c r="S116">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T116">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>36511</v>
+      </c>
+      <c r="B117" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F117" t="s">
+        <v>22</v>
+      </c>
+      <c r="G117">
+        <v>100</v>
+      </c>
+      <c r="H117" t="s">
+        <v>23</v>
+      </c>
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>100</v>
+      </c>
+      <c r="K117">
+        <v>88101</v>
+      </c>
+      <c r="L117" t="s">
+        <v>24</v>
+      </c>
+      <c r="M117">
+        <v>31080</v>
+      </c>
+      <c r="N117" t="s">
+        <v>25</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P117" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R117" t="s">
+        <v>29</v>
+      </c>
+      <c r="S117">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T117">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>36514</v>
+      </c>
+      <c r="B118" t="s">
+        <v>20</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>44.2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>22</v>
+      </c>
+      <c r="G118">
+        <v>122</v>
+      </c>
+      <c r="H118" t="s">
+        <v>23</v>
+      </c>
+      <c r="I118">
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>100</v>
+      </c>
+      <c r="K118">
+        <v>88101</v>
+      </c>
+      <c r="L118" t="s">
+        <v>24</v>
+      </c>
+      <c r="M118">
+        <v>31080</v>
+      </c>
+      <c r="N118" t="s">
+        <v>25</v>
+      </c>
+      <c r="O118" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P118" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q118" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R118" t="s">
+        <v>29</v>
+      </c>
+      <c r="S118">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T118">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>36517</v>
+      </c>
+      <c r="B119" t="s">
+        <v>20</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119">
+        <v>31.2</v>
+      </c>
+      <c r="F119" t="s">
+        <v>22</v>
+      </c>
+      <c r="G119">
+        <v>91</v>
+      </c>
+      <c r="H119" t="s">
+        <v>23</v>
+      </c>
+      <c r="I119">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>100</v>
+      </c>
+      <c r="K119">
+        <v>88101</v>
+      </c>
+      <c r="L119" t="s">
+        <v>24</v>
+      </c>
+      <c r="M119">
+        <v>31080</v>
+      </c>
+      <c r="N119" t="s">
+        <v>25</v>
+      </c>
+      <c r="O119" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P119" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q119" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R119" t="s">
+        <v>29</v>
+      </c>
+      <c r="S119">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T119">
+        <v>-118.21071000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
         <v>36523</v>
       </c>
-      <c r="B111" t="s">
-        <v>20</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111">
-        <v>1</v>
-      </c>
-      <c r="E111">
+      <c r="B120" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
         <v>47.3</v>
       </c>
-      <c r="F111" t="s">
-        <v>22</v>
-      </c>
-      <c r="G111">
+      <c r="F120" t="s">
+        <v>22</v>
+      </c>
+      <c r="G120">
         <v>130</v>
       </c>
-      <c r="H111" t="s">
-        <v>23</v>
-      </c>
-      <c r="I111">
-        <v>1</v>
-      </c>
-      <c r="J111">
-        <v>100</v>
-      </c>
-      <c r="K111">
-        <v>88101</v>
-      </c>
-      <c r="L111" t="s">
-        <v>24</v>
-      </c>
-      <c r="M111">
-        <v>31080</v>
-      </c>
-      <c r="N111" t="s">
-        <v>25</v>
-      </c>
-      <c r="O111" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P111" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q111" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R111" t="s">
-        <v>29</v>
-      </c>
-      <c r="S111">
-        <v>33.928989999999999</v>
-      </c>
-      <c r="T111">
+      <c r="H120" t="s">
+        <v>23</v>
+      </c>
+      <c r="I120">
+        <v>1</v>
+      </c>
+      <c r="J120">
+        <v>100</v>
+      </c>
+      <c r="K120">
+        <v>88101</v>
+      </c>
+      <c r="L120" t="s">
+        <v>24</v>
+      </c>
+      <c r="M120">
+        <v>31080</v>
+      </c>
+      <c r="N120" t="s">
+        <v>25</v>
+      </c>
+      <c r="O120" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P120" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q120" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R120" t="s">
+        <v>29</v>
+      </c>
+      <c r="S120">
+        <v>33.928989999999999</v>
+      </c>
+      <c r="T120">
         <v>-118.21071000000001</v>
       </c>
     </row>

</xml_diff>